<commit_message>
Commit 11/11/2025 #1: 1. Se arreglo el pedo de renombrar, mucho ojo. 2. Se agregaron mas registros apropiados, aun faltan mas
</commit_message>
<xml_diff>
--- a/TAP Tema 1/results/resumen.xlsx
+++ b/TAP Tema 1/results/resumen.xlsx
@@ -177,7 +177,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n" s="0">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="3">
@@ -185,7 +185,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n" s="0">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="4">
@@ -193,7 +193,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n" s="0">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="5">
@@ -201,7 +201,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n" s="0">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="6">
@@ -209,7 +209,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n" s="0">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="7">

</xml_diff>